<commit_message>
Update - creating a new module in 'random_numbers', a computer guess function. What does it mean? - The computer guess the number passed by the user.
</commit_message>
<xml_diff>
--- a/projects/conversoes.xlsx
+++ b/projects/conversoes.xlsx
@@ -416,7 +416,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -509,13 +509,24 @@
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
-        <v>45158.00547519634</v>
+        <v>45158.00547519676</v>
       </c>
       <c r="B8" t="n">
         <v>32</v>
       </c>
       <c r="C8" t="n">
         <v>89.59999999999999</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="n">
+        <v>45158.40210917604</v>
+      </c>
+      <c r="B9" t="n">
+        <v>80</v>
+      </c>
+      <c r="C9" t="n">
+        <v>176</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
CREATE - Weather Forecast Project, using API by OpenWeather. This was also used requests lib and datetime to convert timestamp in real-time formatting
</commit_message>
<xml_diff>
--- a/projects/conversoes.xlsx
+++ b/projects/conversoes.xlsx
@@ -416,7 +416,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -520,13 +520,46 @@
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
-        <v>45158.40210917604</v>
+        <v>45158.40210917824</v>
       </c>
       <c r="B9" t="n">
         <v>80</v>
       </c>
       <c r="C9" t="n">
         <v>176</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="n">
+        <v>45158.51618435185</v>
+      </c>
+      <c r="B10" t="n">
+        <v>30</v>
+      </c>
+      <c r="C10" t="n">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="n">
+        <v>45158.51620192129</v>
+      </c>
+      <c r="B11" t="n">
+        <v>40</v>
+      </c>
+      <c r="C11" t="n">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="n">
+        <v>45158.51622070289</v>
+      </c>
+      <c r="B12" t="n">
+        <v>50</v>
+      </c>
+      <c r="C12" t="n">
+        <v>122</v>
       </c>
     </row>
   </sheetData>

</xml_diff>